<commit_message>
base page building class
</commit_message>
<xml_diff>
--- a/skeleton/layout.xlsx
+++ b/skeleton/layout.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="600" yWindow="30" windowWidth="19395" windowHeight="8955"/>
+    <workbookView xWindow="600" yWindow="45" windowWidth="19395" windowHeight="8940"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -72,6 +72,1223 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95249</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="正方形/長方形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="200025" y="266699"/>
+          <a:ext cx="9601200" cy="12420601"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>95251</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="正方形/長方形 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="200025" y="266701"/>
+          <a:ext cx="9601200" cy="523874"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="正方形/長方形 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="295275" y="323851"/>
+          <a:ext cx="2257425" cy="361949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="lt1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>ロゴ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>42</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152401</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>48</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="正方形/長方形 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8401050" y="323851"/>
+          <a:ext cx="1285875" cy="361949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>ユーザー名</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>49</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>73</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="正方形/長方形 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="200025" y="10572750"/>
+          <a:ext cx="9601200" cy="2105025"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="7" name="正方形/長方形 6"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="333374" y="923925"/>
+          <a:ext cx="2047875" cy="1847850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="8" name="正方形/長方形 7"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2552699" y="923924"/>
+          <a:ext cx="7038976" cy="2305051"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>161923</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="9" name="正方形/長方形 8"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676524" y="1000124"/>
+          <a:ext cx="1285875" cy="361949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>通知</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="10" name="正方形/長方形 9"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2552699" y="3333749"/>
+          <a:ext cx="7038976" cy="2305051"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>152399</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>171448</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="11" name="正方形/長方形 10"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676524" y="3409949"/>
+          <a:ext cx="1285875" cy="361949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>タスク</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>152399</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>133349</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="12" name="正方形/長方形 11"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2552699" y="5791199"/>
+          <a:ext cx="7038976" cy="2305051"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>57148</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="13" name="正方形/長方形 12"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676524" y="5867399"/>
+          <a:ext cx="1285875" cy="361949"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent5">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent5"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent5"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>アクティビティ</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="22" name="正方形/長方形 21"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676524" y="6324600"/>
+          <a:ext cx="6753226" cy="276226"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>通知</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="23" name="正方形/長方形 22"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676524" y="6657975"/>
+          <a:ext cx="6753226" cy="276226"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>通知</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="24" name="正方形/長方形 23"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676524" y="7000875"/>
+          <a:ext cx="6753226" cy="276226"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>通知</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>76201</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="25" name="正方形/長方形 24"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676524" y="7343775"/>
+          <a:ext cx="6753226" cy="276226"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>通知</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>85726</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="26" name="正方形/長方形 25"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676524" y="7696200"/>
+          <a:ext cx="6753226" cy="276226"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>すべて見る</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="33" name="正方形/長方形 32"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676524" y="2847975"/>
+          <a:ext cx="6753226" cy="276226"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>すべて見る</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>38101</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="38" name="正方形/長方形 37"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676524" y="1476375"/>
+          <a:ext cx="6753226" cy="276226"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>通知</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="39" name="正方形/長方形 38"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676524" y="1809750"/>
+          <a:ext cx="6753226" cy="276226"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>通知</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="正方形/長方形 39"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676524" y="2152650"/>
+          <a:ext cx="6753226" cy="276226"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>通知</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>76199</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>47</xdr:col>
+      <xdr:colOff>28575</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>28576</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="41" name="正方形/長方形 40"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2676524" y="2495550"/>
+          <a:ext cx="6753226" cy="276226"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+            <a:t>通知</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -364,13 +1581,14 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" activeCellId="1" sqref="A1 H14"/>
+      <selection activeCell="BD19" sqref="BD19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData/>
   <phoneticPr fontId="1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>